<commit_message>
Started working on graphs and analytics
</commit_message>
<xml_diff>
--- a/ScoutingComplex2015/DataEntry/sample_files/scouting.xlsx
+++ b/ScoutingComplex2015/DataEntry/sample_files/scouting.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="23">
   <si>
     <t>interaction</t>
   </si>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,7 +628,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -676,6 +676,88 @@
         <v>22</v>
       </c>
       <c r="U3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="U5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
began workingwith python to generate graphs
</commit_message>
<xml_diff>
--- a/ScoutingComplex2015/DataEntry/sample_files/scouting.xlsx
+++ b/ScoutingComplex2015/DataEntry/sample_files/scouting.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="24">
   <si>
     <t>interaction</t>
   </si>
@@ -143,15 +143,34 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>binStack</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,13 +193,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,7 +559,8 @@
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="19" width="5.6640625" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="5.6640625" customWidth="1"/>
     <col min="20" max="20" width="8.6640625" customWidth="1"/>
     <col min="21" max="21" width="4.6640625" customWidth="1"/>
   </cols>
@@ -555,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="T1" t="s">
         <v>5</v>
@@ -628,96 +652,93 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
       </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>3</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
       </c>
       <c r="T3" t="s">
         <v>22</v>
       </c>
-      <c r="U3" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="L4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="N4">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T4" t="s">
         <v>22</v>
@@ -725,44 +746,513 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
         <v>22</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="K5">
+        <v>23</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>23</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9">
         <v>12</v>
       </c>
-      <c r="L5">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>12</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <v>18</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>14</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12">
+        <v>17</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>16</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
         <v>2</v>
       </c>
-      <c r="R5">
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13">
+        <v>18</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>20</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
         <v>3</v>
       </c>
-      <c r="S5">
-        <v>4</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="T13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>